<commit_message>
reconnect to github remote
</commit_message>
<xml_diff>
--- a/明正國小確診通報.xlsx
+++ b/明正國小確診通報.xlsx
@@ -1183,7 +1183,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AN11"/>
+  <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView showGridLines="0" defaultGridColor="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1208,8 +1208,8 @@
     <col width="16.3516" customWidth="1" style="1" min="17" max="17"/>
     <col width="15.8516" customWidth="1" style="1" min="18" max="18"/>
     <col width="19.3516" customWidth="1" style="1" min="19" max="19"/>
-    <col width="18.8516" customWidth="1" style="1" min="20" max="40"/>
-    <col width="12.6719" customWidth="1" style="1" min="41" max="16384"/>
+    <col width="18.8516" customWidth="1" style="1" min="20" max="44"/>
+    <col width="12.6719" customWidth="1" style="1" min="45" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1" s="6">
@@ -1230,17 +1230,17 @@
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>潘竑杰</t>
+          <t>江宥囿</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>一年級</t>
+          <t>二年級</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>乙班</t>
+          <t>庚班</t>
         </is>
       </c>
       <c r="G1" s="4" t="n">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>導師通報：同住爸爸、阿公、阿嬤皆快篩陽。學童目前快篩陰。</t>
+          <t>同住阿嬤確診6/23</t>
         </is>
       </c>
       <c r="K1" s="4" t="n"/>
@@ -1288,9 +1288,39 @@
       <c r="AI1" s="4" t="n"/>
       <c r="AJ1" s="4" t="n"/>
       <c r="AK1" s="4" t="n"/>
-      <c r="AL1" s="4" t="n"/>
-      <c r="AM1" s="4" t="n"/>
-      <c r="AN1" s="4" t="n"/>
+      <c r="AL1" s="2" t="inlineStr">
+        <is>
+          <t>2022/6/26 下午 2:01:45</t>
+        </is>
+      </c>
+      <c r="AM1" s="2" t="inlineStr">
+        <is>
+          <t>首次通報</t>
+        </is>
+      </c>
+      <c r="AN1" s="2" t="inlineStr">
+        <is>
+          <t>學生</t>
+        </is>
+      </c>
+      <c r="AO1" s="2" t="inlineStr">
+        <is>
+          <t>江宥囿</t>
+        </is>
+      </c>
+      <c r="AP1" s="2" t="inlineStr">
+        <is>
+          <t>二年級</t>
+        </is>
+      </c>
+      <c r="AQ1" s="2" t="inlineStr">
+        <is>
+          <t>庚班</t>
+        </is>
+      </c>
+      <c r="AR1" s="4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1" s="6">
       <c r="A2" s="2" t="inlineStr">
@@ -1310,25 +1340,25 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>梁哲豪</t>
+          <t>陳琳媛</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>六年級</t>
+          <t>三年級</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>丁班</t>
+          <t>戊班</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>疑似確診</t>
+          <t>快篩陽</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
@@ -1336,11 +1366,7 @@
           <t>在家中</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>導師通報：學童媽媽昨日6/14確診，學童目前無症狀，未快篩。已告知導師明天畢業典禮勿到校。</t>
-        </is>
-      </c>
+      <c r="J2" s="4" t="n"/>
       <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="4" t="n"/>
@@ -1368,20 +1394,84 @@
       <c r="AI2" s="4" t="n"/>
       <c r="AJ2" s="4" t="n"/>
       <c r="AK2" s="4" t="n"/>
-      <c r="AL2" s="4" t="n"/>
-      <c r="AM2" s="4" t="n"/>
-      <c r="AN2" s="4" t="n"/>
+      <c r="AL2" s="2" t="inlineStr">
+        <is>
+          <t>2022/6/26 下午 3:14:34</t>
+        </is>
+      </c>
+      <c r="AM2" s="2" t="inlineStr">
+        <is>
+          <t>首次通報</t>
+        </is>
+      </c>
+      <c r="AN2" s="2" t="inlineStr">
+        <is>
+          <t>學生</t>
+        </is>
+      </c>
+      <c r="AO2" s="2" t="inlineStr">
+        <is>
+          <t>陳琳媛</t>
+        </is>
+      </c>
+      <c r="AP2" s="2" t="inlineStr">
+        <is>
+          <t>三年級</t>
+        </is>
+      </c>
+      <c r="AQ2" s="2" t="inlineStr">
+        <is>
+          <t>戊班</t>
+        </is>
+      </c>
+      <c r="AR2" s="4" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" ht="13.65" customHeight="1" s="6">
-      <c r="A3" s="4" t="n"/>
-      <c r="B3" s="4" t="n"/>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="2" t="n"/>
-      <c r="E3" s="4" t="n"/>
-      <c r="F3" s="4" t="n"/>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="4" t="n"/>
-      <c r="I3" s="4" t="n"/>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>該筆資料ok</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>首次通報</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>學生</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>吳承翰</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>四年級</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>甲班</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>快篩陽</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>在家中</t>
+        </is>
+      </c>
       <c r="J3" s="4" t="n"/>
       <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
@@ -1410,21 +1500,89 @@
       <c r="AI3" s="4" t="n"/>
       <c r="AJ3" s="4" t="n"/>
       <c r="AK3" s="4" t="n"/>
-      <c r="AL3" s="4" t="n"/>
-      <c r="AM3" s="4" t="n"/>
-      <c r="AN3" s="4" t="n"/>
+      <c r="AL3" s="2" t="inlineStr">
+        <is>
+          <t>2022/6/26 下午 7:49:07</t>
+        </is>
+      </c>
+      <c r="AM3" s="2" t="inlineStr">
+        <is>
+          <t>首次通報</t>
+        </is>
+      </c>
+      <c r="AN3" s="2" t="inlineStr">
+        <is>
+          <t>學生</t>
+        </is>
+      </c>
+      <c r="AO3" s="2" t="inlineStr">
+        <is>
+          <t>吳承翰</t>
+        </is>
+      </c>
+      <c r="AP3" s="2" t="inlineStr">
+        <is>
+          <t>四年級</t>
+        </is>
+      </c>
+      <c r="AQ3" s="2" t="inlineStr">
+        <is>
+          <t>甲班</t>
+        </is>
+      </c>
+      <c r="AR3" s="4" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" ht="13.65" customHeight="1" s="6">
-      <c r="A4" s="7" t="n"/>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" s="2" t="n"/>
-      <c r="G4" s="4" t="n"/>
-      <c r="H4" s="2" t="n"/>
-      <c r="I4" s="2" t="n"/>
-      <c r="J4" s="2" t="n"/>
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>該筆資料ok</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>首次通報</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>學生</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>江宥囿</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>二年級</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>庚班</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>疑似確診</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>在家中</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>同住阿嬤確診6/23</t>
+        </is>
+      </c>
       <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="4" t="n"/>
@@ -1452,9 +1610,37 @@
       <c r="AI4" s="4" t="n"/>
       <c r="AJ4" s="4" t="n"/>
       <c r="AK4" s="4" t="n"/>
-      <c r="AL4" s="4" t="n"/>
-      <c r="AM4" s="4" t="n"/>
-      <c r="AN4" s="4" t="n"/>
+      <c r="AL4" s="7" t="n">
+        <v>44738.58454861111</v>
+      </c>
+      <c r="AM4" s="2" t="inlineStr">
+        <is>
+          <t>首次通報</t>
+        </is>
+      </c>
+      <c r="AN4" s="2" t="inlineStr">
+        <is>
+          <t>學生</t>
+        </is>
+      </c>
+      <c r="AO4" s="2" t="inlineStr">
+        <is>
+          <t>江宥囿</t>
+        </is>
+      </c>
+      <c r="AP4" s="2" t="inlineStr">
+        <is>
+          <t>二年級</t>
+        </is>
+      </c>
+      <c r="AQ4" s="2" t="inlineStr">
+        <is>
+          <t>庚班</t>
+        </is>
+      </c>
+      <c r="AR4" s="4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" ht="13.65" customHeight="1" s="6">
       <c r="A5" s="4" t="n"/>
@@ -1497,6 +1683,10 @@
       <c r="AL5" s="4" t="n"/>
       <c r="AM5" s="4" t="n"/>
       <c r="AN5" s="4" t="n"/>
+      <c r="AO5" s="4" t="n"/>
+      <c r="AP5" s="4" t="n"/>
+      <c r="AQ5" s="4" t="n"/>
+      <c r="AR5" s="4" t="n"/>
     </row>
     <row r="6" ht="13.65" customHeight="1" s="6">
       <c r="A6" s="4" t="n"/>
@@ -1539,6 +1729,10 @@
       <c r="AL6" s="4" t="n"/>
       <c r="AM6" s="4" t="n"/>
       <c r="AN6" s="4" t="n"/>
+      <c r="AO6" s="4" t="n"/>
+      <c r="AP6" s="4" t="n"/>
+      <c r="AQ6" s="4" t="n"/>
+      <c r="AR6" s="4" t="n"/>
     </row>
     <row r="7" ht="13.65" customHeight="1" s="6">
       <c r="A7" s="4" t="n"/>
@@ -1581,6 +1775,10 @@
       <c r="AL7" s="4" t="n"/>
       <c r="AM7" s="4" t="n"/>
       <c r="AN7" s="4" t="n"/>
+      <c r="AO7" s="4" t="n"/>
+      <c r="AP7" s="4" t="n"/>
+      <c r="AQ7" s="4" t="n"/>
+      <c r="AR7" s="4" t="n"/>
     </row>
     <row r="8" ht="13.65" customHeight="1" s="6">
       <c r="A8" s="4" t="n"/>
@@ -1623,6 +1821,10 @@
       <c r="AL8" s="4" t="n"/>
       <c r="AM8" s="4" t="n"/>
       <c r="AN8" s="4" t="n"/>
+      <c r="AO8" s="4" t="n"/>
+      <c r="AP8" s="4" t="n"/>
+      <c r="AQ8" s="4" t="n"/>
+      <c r="AR8" s="4" t="n"/>
     </row>
     <row r="9" ht="13.65" customHeight="1" s="6">
       <c r="A9" s="4" t="n"/>
@@ -1665,6 +1867,10 @@
       <c r="AL9" s="4" t="n"/>
       <c r="AM9" s="4" t="n"/>
       <c r="AN9" s="4" t="n"/>
+      <c r="AO9" s="4" t="n"/>
+      <c r="AP9" s="4" t="n"/>
+      <c r="AQ9" s="4" t="n"/>
+      <c r="AR9" s="4" t="n"/>
     </row>
     <row r="10" ht="13.65" customHeight="1" s="6">
       <c r="A10" s="4" t="n"/>
@@ -1707,6 +1913,10 @@
       <c r="AL10" s="4" t="n"/>
       <c r="AM10" s="4" t="n"/>
       <c r="AN10" s="4" t="n"/>
+      <c r="AO10" s="4" t="n"/>
+      <c r="AP10" s="4" t="n"/>
+      <c r="AQ10" s="4" t="n"/>
+      <c r="AR10" s="4" t="n"/>
     </row>
     <row r="11" ht="13.65" customHeight="1" s="6">
       <c r="A11" s="4" t="n"/>
@@ -1749,6 +1959,10 @@
       <c r="AL11" s="4" t="n"/>
       <c r="AM11" s="4" t="n"/>
       <c r="AN11" s="4" t="n"/>
+      <c r="AO11" s="4" t="n"/>
+      <c r="AP11" s="4" t="n"/>
+      <c r="AQ11" s="4" t="n"/>
+      <c r="AR11" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>